<commit_message>
chore: update PRODOC rubric spreadsheet
</commit_message>
<xml_diff>
--- a/PRODOC_rubric.xlsx
+++ b/PRODOC_rubric.xlsx
@@ -24,7 +24,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="170">
   <si>
-    <t xml:space="preserve">Dimension</t>
+    <t xml:space="preserve">Dimensión</t>
   </si>
   <si>
     <t xml:space="preserve">Criterio</t>
@@ -5353,7 +5353,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5363,15 +5363,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -5406,31 +5398,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5633,9 +5609,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1021680</xdr:colOff>
+      <xdr:colOff>1021320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5649,7 +5625,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="104760" y="66600"/>
-          <a:ext cx="916920" cy="597960"/>
+          <a:ext cx="916560" cy="597600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5779,567 +5755,566 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="28.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="30.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="3" width="60"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="4" width="11.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="28.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="30.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="2" width="60"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="8" style="1" width="11.45"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="143.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="138.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="207.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="201.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="104.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="101.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="220.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="213.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="130.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="126.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="233.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="226.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="181.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="117.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="113.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="194.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="188.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="65.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="63.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="168.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="163.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="143.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="138.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="298.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="288.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="233.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="226.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="233.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="226.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="362.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="351.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="143.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="138.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="G18" s="15" t="s">
+      <c r="G18" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="168.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="163.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="156.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="151.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="10" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="156.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="151.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="104.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="101.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="194.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="188.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="168.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="163.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="7" t="s">
         <v>131</v>
       </c>
     </row>
@@ -6362,1256 +6337,1256 @@
   <dimension ref="A2:L257"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="28.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="15.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="5.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="60"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="20" width="28.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="20" width="32.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="21" width="21.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="20" width="32.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="34.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="20" width="32.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="14" width="28.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="14" width="15.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="14" width="5.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="14" width="56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="14" width="60"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="14" width="28.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="14" width="32.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="15" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="14" width="32.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="34.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="14" width="32.73"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="24.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="25"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="68.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="20"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="110" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="20"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="20"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="101.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="F13" s="39" t="s">
+      <c r="F13" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="20"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="20"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="194" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="F15" s="39" t="s">
+      <c r="F15" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="20"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="188.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="40" t="s">
         <v>164</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="F16" s="39" t="s">
+      <c r="F16" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="20"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="20"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="251.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="20"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="14"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I19" s="47"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I21" s="47"/>
-      <c r="J21" s="48"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="42"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I22" s="47"/>
-      <c r="J22" s="48"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="42"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I23" s="47"/>
-      <c r="J23" s="48"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="42"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I24" s="47"/>
-      <c r="J24" s="48"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="42"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I25" s="47"/>
-      <c r="J25" s="48"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="42"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I26" s="47"/>
-      <c r="J26" s="48"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="42"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I27" s="47"/>
-      <c r="J27" s="48"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I28" s="47"/>
-      <c r="J28" s="48"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I29" s="47"/>
-      <c r="J29" s="48"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="42"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I30" s="47"/>
-      <c r="J30" s="48"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="42"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I31" s="47"/>
-      <c r="J31" s="48"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="42"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I32" s="47"/>
-      <c r="J32" s="48"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="42"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I33" s="47"/>
-      <c r="J33" s="48"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="42"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I34" s="47"/>
-      <c r="J34" s="48"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="42"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I35" s="47"/>
-      <c r="J35" s="48"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="42"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I36" s="47"/>
-      <c r="J36" s="48"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="42"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I37" s="47"/>
-      <c r="J37" s="48"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="42"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I38" s="47"/>
-      <c r="J38" s="48"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="42"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I39" s="47"/>
-      <c r="J39" s="48"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="42"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I40" s="47"/>
-      <c r="J40" s="48"/>
+      <c r="I40" s="41"/>
+      <c r="J40" s="42"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I41" s="47"/>
-      <c r="J41" s="48"/>
+      <c r="I41" s="41"/>
+      <c r="J41" s="42"/>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I42" s="47"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="42"/>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I43" s="47"/>
-      <c r="J43" s="48"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="42"/>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I44" s="47"/>
-      <c r="J44" s="48"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="42"/>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I45" s="47"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="42"/>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I46" s="47"/>
-      <c r="J46" s="48"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="42"/>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I47" s="47"/>
-      <c r="J47" s="48"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="42"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I48" s="47"/>
-      <c r="J48" s="48"/>
+      <c r="I48" s="41"/>
+      <c r="J48" s="42"/>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I49" s="47"/>
-      <c r="J49" s="48"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="42"/>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I50" s="47"/>
-      <c r="J50" s="48"/>
+      <c r="I50" s="41"/>
+      <c r="J50" s="42"/>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I51" s="47"/>
-      <c r="J51" s="48"/>
+      <c r="I51" s="41"/>
+      <c r="J51" s="42"/>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I52" s="47"/>
-      <c r="J52" s="48"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="42"/>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I53" s="47"/>
-      <c r="J53" s="48"/>
+      <c r="I53" s="41"/>
+      <c r="J53" s="42"/>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I54" s="47"/>
-      <c r="J54" s="48"/>
+      <c r="I54" s="41"/>
+      <c r="J54" s="42"/>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I55" s="47"/>
-      <c r="J55" s="48"/>
+      <c r="I55" s="41"/>
+      <c r="J55" s="42"/>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I56" s="47"/>
-      <c r="J56" s="48"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="42"/>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I57" s="47"/>
-      <c r="J57" s="48"/>
+      <c r="I57" s="41"/>
+      <c r="J57" s="42"/>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I58" s="47"/>
-      <c r="J58" s="48"/>
+      <c r="I58" s="41"/>
+      <c r="J58" s="42"/>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I59" s="47"/>
-      <c r="J59" s="48"/>
+      <c r="I59" s="41"/>
+      <c r="J59" s="42"/>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I60" s="47"/>
-      <c r="J60" s="48"/>
+      <c r="I60" s="41"/>
+      <c r="J60" s="42"/>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I61" s="47"/>
-      <c r="J61" s="48"/>
+      <c r="I61" s="41"/>
+      <c r="J61" s="42"/>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I62" s="47"/>
-      <c r="J62" s="48"/>
+      <c r="I62" s="41"/>
+      <c r="J62" s="42"/>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I63" s="47"/>
-      <c r="J63" s="48"/>
+      <c r="I63" s="41"/>
+      <c r="J63" s="42"/>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I64" s="47"/>
-      <c r="J64" s="48"/>
+      <c r="I64" s="41"/>
+      <c r="J64" s="42"/>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I65" s="47"/>
-      <c r="J65" s="48"/>
+      <c r="I65" s="41"/>
+      <c r="J65" s="42"/>
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I66" s="47"/>
-      <c r="J66" s="48"/>
+      <c r="I66" s="41"/>
+      <c r="J66" s="42"/>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I67" s="47"/>
-      <c r="J67" s="48"/>
+      <c r="I67" s="41"/>
+      <c r="J67" s="42"/>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I68" s="47"/>
-      <c r="J68" s="48"/>
+      <c r="I68" s="41"/>
+      <c r="J68" s="42"/>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I69" s="47"/>
-      <c r="J69" s="48"/>
+      <c r="I69" s="41"/>
+      <c r="J69" s="42"/>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I70" s="47"/>
-      <c r="J70" s="48"/>
+      <c r="I70" s="41"/>
+      <c r="J70" s="42"/>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I71" s="47"/>
-      <c r="J71" s="48"/>
+      <c r="I71" s="41"/>
+      <c r="J71" s="42"/>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I72" s="47"/>
-      <c r="J72" s="48"/>
+      <c r="I72" s="41"/>
+      <c r="J72" s="42"/>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I73" s="47"/>
-      <c r="J73" s="48"/>
+      <c r="I73" s="41"/>
+      <c r="J73" s="42"/>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I74" s="47"/>
-      <c r="J74" s="48"/>
+      <c r="I74" s="41"/>
+      <c r="J74" s="42"/>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I75" s="47"/>
-      <c r="J75" s="48"/>
+      <c r="I75" s="41"/>
+      <c r="J75" s="42"/>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I76" s="47"/>
-      <c r="J76" s="48"/>
+      <c r="I76" s="41"/>
+      <c r="J76" s="42"/>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I77" s="47"/>
-      <c r="J77" s="48"/>
+      <c r="I77" s="41"/>
+      <c r="J77" s="42"/>
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I78" s="47"/>
-      <c r="J78" s="48"/>
+      <c r="I78" s="41"/>
+      <c r="J78" s="42"/>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I79" s="47"/>
-      <c r="J79" s="48"/>
+      <c r="I79" s="41"/>
+      <c r="J79" s="42"/>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I80" s="47"/>
-      <c r="J80" s="48"/>
+      <c r="I80" s="41"/>
+      <c r="J80" s="42"/>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I81" s="47"/>
-      <c r="J81" s="48"/>
+      <c r="I81" s="41"/>
+      <c r="J81" s="42"/>
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I82" s="47"/>
-      <c r="J82" s="48"/>
+      <c r="I82" s="41"/>
+      <c r="J82" s="42"/>
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I83" s="47"/>
-      <c r="J83" s="48"/>
+      <c r="I83" s="41"/>
+      <c r="J83" s="42"/>
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I84" s="47"/>
-      <c r="J84" s="48"/>
+      <c r="I84" s="41"/>
+      <c r="J84" s="42"/>
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I85" s="47"/>
-      <c r="J85" s="48"/>
+      <c r="I85" s="41"/>
+      <c r="J85" s="42"/>
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I86" s="47"/>
-      <c r="J86" s="48"/>
+      <c r="I86" s="41"/>
+      <c r="J86" s="42"/>
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I87" s="47"/>
-      <c r="J87" s="48"/>
+      <c r="I87" s="41"/>
+      <c r="J87" s="42"/>
     </row>
     <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I88" s="47"/>
-      <c r="J88" s="48"/>
+      <c r="I88" s="41"/>
+      <c r="J88" s="42"/>
     </row>
     <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I89" s="47"/>
-      <c r="J89" s="48"/>
+      <c r="I89" s="41"/>
+      <c r="J89" s="42"/>
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I90" s="47"/>
-      <c r="J90" s="48"/>
+      <c r="I90" s="41"/>
+      <c r="J90" s="42"/>
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I91" s="47"/>
-      <c r="J91" s="48"/>
+      <c r="I91" s="41"/>
+      <c r="J91" s="42"/>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I92" s="47"/>
-      <c r="J92" s="48"/>
+      <c r="I92" s="41"/>
+      <c r="J92" s="42"/>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I93" s="47"/>
-      <c r="J93" s="48"/>
+      <c r="I93" s="41"/>
+      <c r="J93" s="42"/>
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I94" s="47"/>
-      <c r="J94" s="48"/>
+      <c r="I94" s="41"/>
+      <c r="J94" s="42"/>
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I95" s="47"/>
-      <c r="J95" s="48"/>
+      <c r="I95" s="41"/>
+      <c r="J95" s="42"/>
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I96" s="47"/>
-      <c r="J96" s="48"/>
+      <c r="I96" s="41"/>
+      <c r="J96" s="42"/>
     </row>
     <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I97" s="47"/>
-      <c r="J97" s="48"/>
+      <c r="I97" s="41"/>
+      <c r="J97" s="42"/>
     </row>
     <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I98" s="47"/>
-      <c r="J98" s="48"/>
+      <c r="I98" s="41"/>
+      <c r="J98" s="42"/>
     </row>
     <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I99" s="47"/>
-      <c r="J99" s="48"/>
+      <c r="I99" s="41"/>
+      <c r="J99" s="42"/>
     </row>
     <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I100" s="47"/>
-      <c r="J100" s="48"/>
+      <c r="I100" s="41"/>
+      <c r="J100" s="42"/>
     </row>
     <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I101" s="47"/>
-      <c r="J101" s="48"/>
+      <c r="I101" s="41"/>
+      <c r="J101" s="42"/>
     </row>
     <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I102" s="47"/>
-      <c r="J102" s="48"/>
+      <c r="I102" s="41"/>
+      <c r="J102" s="42"/>
     </row>
     <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I103" s="47"/>
-      <c r="J103" s="48"/>
+      <c r="I103" s="41"/>
+      <c r="J103" s="42"/>
     </row>
     <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I104" s="47"/>
-      <c r="J104" s="48"/>
+      <c r="I104" s="41"/>
+      <c r="J104" s="42"/>
     </row>
     <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I105" s="47"/>
-      <c r="J105" s="48"/>
+      <c r="I105" s="41"/>
+      <c r="J105" s="42"/>
     </row>
     <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I106" s="47"/>
-      <c r="J106" s="48"/>
+      <c r="I106" s="41"/>
+      <c r="J106" s="42"/>
     </row>
     <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I107" s="47"/>
-      <c r="J107" s="48"/>
+      <c r="I107" s="41"/>
+      <c r="J107" s="42"/>
     </row>
     <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I108" s="47"/>
-      <c r="J108" s="48"/>
+      <c r="I108" s="41"/>
+      <c r="J108" s="42"/>
     </row>
     <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I109" s="47"/>
-      <c r="J109" s="48"/>
+      <c r="I109" s="41"/>
+      <c r="J109" s="42"/>
     </row>
     <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I110" s="47"/>
-      <c r="J110" s="48"/>
+      <c r="I110" s="41"/>
+      <c r="J110" s="42"/>
     </row>
     <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I111" s="47"/>
-      <c r="J111" s="48"/>
+      <c r="I111" s="41"/>
+      <c r="J111" s="42"/>
     </row>
     <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I112" s="47"/>
-      <c r="J112" s="48"/>
+      <c r="I112" s="41"/>
+      <c r="J112" s="42"/>
     </row>
     <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I113" s="47"/>
-      <c r="J113" s="48"/>
+      <c r="I113" s="41"/>
+      <c r="J113" s="42"/>
     </row>
     <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I114" s="47"/>
-      <c r="J114" s="48"/>
+      <c r="I114" s="41"/>
+      <c r="J114" s="42"/>
     </row>
     <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I115" s="47"/>
-      <c r="J115" s="48"/>
+      <c r="I115" s="41"/>
+      <c r="J115" s="42"/>
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I116" s="47"/>
-      <c r="J116" s="48"/>
+      <c r="I116" s="41"/>
+      <c r="J116" s="42"/>
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I117" s="47"/>
-      <c r="J117" s="48"/>
+      <c r="I117" s="41"/>
+      <c r="J117" s="42"/>
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I118" s="47"/>
-      <c r="J118" s="48"/>
+      <c r="I118" s="41"/>
+      <c r="J118" s="42"/>
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I119" s="47"/>
-      <c r="J119" s="48"/>
+      <c r="I119" s="41"/>
+      <c r="J119" s="42"/>
     </row>
     <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I120" s="47"/>
-      <c r="J120" s="48"/>
+      <c r="I120" s="41"/>
+      <c r="J120" s="42"/>
     </row>
     <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I121" s="47"/>
-      <c r="J121" s="48"/>
+      <c r="I121" s="41"/>
+      <c r="J121" s="42"/>
     </row>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I122" s="47"/>
-      <c r="J122" s="48"/>
+      <c r="I122" s="41"/>
+      <c r="J122" s="42"/>
     </row>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I123" s="47"/>
-      <c r="J123" s="48"/>
+      <c r="I123" s="41"/>
+      <c r="J123" s="42"/>
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I124" s="47"/>
-      <c r="J124" s="48"/>
+      <c r="I124" s="41"/>
+      <c r="J124" s="42"/>
     </row>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I125" s="47"/>
-      <c r="J125" s="48"/>
+      <c r="I125" s="41"/>
+      <c r="J125" s="42"/>
     </row>
     <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I126" s="47"/>
-      <c r="J126" s="48"/>
+      <c r="I126" s="41"/>
+      <c r="J126" s="42"/>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I127" s="47"/>
-      <c r="J127" s="48"/>
+      <c r="I127" s="41"/>
+      <c r="J127" s="42"/>
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I128" s="47"/>
-      <c r="J128" s="48"/>
+      <c r="I128" s="41"/>
+      <c r="J128" s="42"/>
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I129" s="47"/>
-      <c r="J129" s="48"/>
+      <c r="I129" s="41"/>
+      <c r="J129" s="42"/>
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I130" s="47"/>
-      <c r="J130" s="48"/>
+      <c r="I130" s="41"/>
+      <c r="J130" s="42"/>
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I131" s="47"/>
-      <c r="J131" s="48"/>
+      <c r="I131" s="41"/>
+      <c r="J131" s="42"/>
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I132" s="47"/>
-      <c r="J132" s="48"/>
+      <c r="I132" s="41"/>
+      <c r="J132" s="42"/>
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I133" s="47"/>
-      <c r="J133" s="48"/>
+      <c r="I133" s="41"/>
+      <c r="J133" s="42"/>
     </row>
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I134" s="47"/>
-      <c r="J134" s="48"/>
+      <c r="I134" s="41"/>
+      <c r="J134" s="42"/>
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I135" s="47"/>
-      <c r="J135" s="48"/>
+      <c r="I135" s="41"/>
+      <c r="J135" s="42"/>
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I136" s="47"/>
-      <c r="J136" s="48"/>
+      <c r="I136" s="41"/>
+      <c r="J136" s="42"/>
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I137" s="47"/>
-      <c r="J137" s="48"/>
+      <c r="I137" s="41"/>
+      <c r="J137" s="42"/>
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I138" s="47"/>
-      <c r="J138" s="48"/>
+      <c r="I138" s="41"/>
+      <c r="J138" s="42"/>
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I139" s="47"/>
-      <c r="J139" s="48"/>
+      <c r="I139" s="41"/>
+      <c r="J139" s="42"/>
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I140" s="47"/>
-      <c r="J140" s="48"/>
+      <c r="I140" s="41"/>
+      <c r="J140" s="42"/>
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I141" s="47"/>
-      <c r="J141" s="48"/>
+      <c r="I141" s="41"/>
+      <c r="J141" s="42"/>
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I142" s="47"/>
-      <c r="J142" s="48"/>
+      <c r="I142" s="41"/>
+      <c r="J142" s="42"/>
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I143" s="47"/>
-      <c r="J143" s="48"/>
+      <c r="I143" s="41"/>
+      <c r="J143" s="42"/>
     </row>
     <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I144" s="47"/>
-      <c r="J144" s="48"/>
+      <c r="I144" s="41"/>
+      <c r="J144" s="42"/>
     </row>
     <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I145" s="47"/>
-      <c r="J145" s="48"/>
+      <c r="I145" s="41"/>
+      <c r="J145" s="42"/>
     </row>
     <row r="146" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I146" s="47"/>
-      <c r="J146" s="48"/>
+      <c r="I146" s="41"/>
+      <c r="J146" s="42"/>
     </row>
     <row r="147" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I147" s="47"/>
-      <c r="J147" s="48"/>
+      <c r="I147" s="41"/>
+      <c r="J147" s="42"/>
     </row>
     <row r="148" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I148" s="47"/>
-      <c r="J148" s="48"/>
+      <c r="I148" s="41"/>
+      <c r="J148" s="42"/>
     </row>
     <row r="149" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I149" s="47"/>
-      <c r="J149" s="48"/>
+      <c r="I149" s="41"/>
+      <c r="J149" s="42"/>
     </row>
     <row r="150" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I150" s="47"/>
-      <c r="J150" s="48"/>
+      <c r="I150" s="41"/>
+      <c r="J150" s="42"/>
     </row>
     <row r="151" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I151" s="47"/>
-      <c r="J151" s="48"/>
+      <c r="I151" s="41"/>
+      <c r="J151" s="42"/>
     </row>
     <row r="152" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I152" s="47"/>
-      <c r="J152" s="48"/>
+      <c r="I152" s="41"/>
+      <c r="J152" s="42"/>
     </row>
     <row r="153" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I153" s="47"/>
-      <c r="J153" s="48"/>
+      <c r="I153" s="41"/>
+      <c r="J153" s="42"/>
     </row>
     <row r="154" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I154" s="47"/>
-      <c r="J154" s="48"/>
+      <c r="I154" s="41"/>
+      <c r="J154" s="42"/>
     </row>
     <row r="155" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I155" s="47"/>
-      <c r="J155" s="48"/>
+      <c r="I155" s="41"/>
+      <c r="J155" s="42"/>
     </row>
     <row r="156" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I156" s="47"/>
-      <c r="J156" s="48"/>
+      <c r="I156" s="41"/>
+      <c r="J156" s="42"/>
     </row>
     <row r="157" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I157" s="47"/>
-      <c r="J157" s="48"/>
+      <c r="I157" s="41"/>
+      <c r="J157" s="42"/>
     </row>
     <row r="158" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I158" s="47"/>
-      <c r="J158" s="48"/>
+      <c r="I158" s="41"/>
+      <c r="J158" s="42"/>
     </row>
     <row r="159" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I159" s="47"/>
-      <c r="J159" s="48"/>
+      <c r="I159" s="41"/>
+      <c r="J159" s="42"/>
     </row>
     <row r="160" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I160" s="47"/>
-      <c r="J160" s="48"/>
+      <c r="I160" s="41"/>
+      <c r="J160" s="42"/>
     </row>
     <row r="161" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I161" s="47"/>
-      <c r="J161" s="48"/>
+      <c r="I161" s="41"/>
+      <c r="J161" s="42"/>
     </row>
     <row r="162" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I162" s="47"/>
-      <c r="J162" s="48"/>
+      <c r="I162" s="41"/>
+      <c r="J162" s="42"/>
     </row>
     <row r="163" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I163" s="47"/>
-      <c r="J163" s="48"/>
+      <c r="I163" s="41"/>
+      <c r="J163" s="42"/>
     </row>
     <row r="164" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I164" s="47"/>
-      <c r="J164" s="48"/>
+      <c r="I164" s="41"/>
+      <c r="J164" s="42"/>
     </row>
     <row r="165" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I165" s="47"/>
-      <c r="J165" s="48"/>
+      <c r="I165" s="41"/>
+      <c r="J165" s="42"/>
     </row>
     <row r="166" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I166" s="47"/>
-      <c r="J166" s="48"/>
+      <c r="I166" s="41"/>
+      <c r="J166" s="42"/>
     </row>
     <row r="167" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I167" s="47"/>
-      <c r="J167" s="48"/>
+      <c r="I167" s="41"/>
+      <c r="J167" s="42"/>
     </row>
     <row r="168" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I168" s="47"/>
-      <c r="J168" s="48"/>
+      <c r="I168" s="41"/>
+      <c r="J168" s="42"/>
     </row>
     <row r="169" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I169" s="47"/>
-      <c r="J169" s="48"/>
+      <c r="I169" s="41"/>
+      <c r="J169" s="42"/>
     </row>
     <row r="170" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I170" s="47"/>
-      <c r="J170" s="48"/>
+      <c r="I170" s="41"/>
+      <c r="J170" s="42"/>
     </row>
     <row r="171" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I171" s="47"/>
-      <c r="J171" s="48"/>
+      <c r="I171" s="41"/>
+      <c r="J171" s="42"/>
     </row>
     <row r="172" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I172" s="47"/>
-      <c r="J172" s="48"/>
+      <c r="I172" s="41"/>
+      <c r="J172" s="42"/>
     </row>
     <row r="173" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I173" s="47"/>
-      <c r="J173" s="48"/>
+      <c r="I173" s="41"/>
+      <c r="J173" s="42"/>
     </row>
     <row r="174" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I174" s="47"/>
-      <c r="J174" s="48"/>
+      <c r="I174" s="41"/>
+      <c r="J174" s="42"/>
     </row>
     <row r="175" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I175" s="47"/>
-      <c r="J175" s="48"/>
+      <c r="I175" s="41"/>
+      <c r="J175" s="42"/>
     </row>
     <row r="176" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I176" s="47"/>
-      <c r="J176" s="48"/>
+      <c r="I176" s="41"/>
+      <c r="J176" s="42"/>
     </row>
     <row r="177" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I177" s="47"/>
-      <c r="J177" s="48"/>
+      <c r="I177" s="41"/>
+      <c r="J177" s="42"/>
     </row>
     <row r="178" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I178" s="47"/>
-      <c r="J178" s="48"/>
+      <c r="I178" s="41"/>
+      <c r="J178" s="42"/>
     </row>
     <row r="179" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I179" s="47"/>
-      <c r="J179" s="48"/>
+      <c r="I179" s="41"/>
+      <c r="J179" s="42"/>
     </row>
     <row r="180" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I180" s="47"/>
-      <c r="J180" s="48"/>
+      <c r="I180" s="41"/>
+      <c r="J180" s="42"/>
     </row>
     <row r="181" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I181" s="47"/>
-      <c r="J181" s="48"/>
+      <c r="I181" s="41"/>
+      <c r="J181" s="42"/>
     </row>
     <row r="182" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I182" s="47"/>
-      <c r="J182" s="48"/>
+      <c r="I182" s="41"/>
+      <c r="J182" s="42"/>
     </row>
     <row r="183" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I183" s="47"/>
-      <c r="J183" s="48"/>
+      <c r="I183" s="41"/>
+      <c r="J183" s="42"/>
     </row>
     <row r="184" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I184" s="47"/>
-      <c r="J184" s="48"/>
+      <c r="I184" s="41"/>
+      <c r="J184" s="42"/>
     </row>
     <row r="185" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I185" s="47"/>
-      <c r="J185" s="48"/>
+      <c r="I185" s="41"/>
+      <c r="J185" s="42"/>
     </row>
     <row r="186" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I186" s="47"/>
-      <c r="J186" s="48"/>
+      <c r="I186" s="41"/>
+      <c r="J186" s="42"/>
     </row>
     <row r="187" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I187" s="47"/>
-      <c r="J187" s="48"/>
+      <c r="I187" s="41"/>
+      <c r="J187" s="42"/>
     </row>
     <row r="188" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I188" s="47"/>
-      <c r="J188" s="48"/>
+      <c r="I188" s="41"/>
+      <c r="J188" s="42"/>
     </row>
     <row r="189" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I189" s="47"/>
-      <c r="J189" s="48"/>
+      <c r="I189" s="41"/>
+      <c r="J189" s="42"/>
     </row>
     <row r="190" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I190" s="47"/>
-      <c r="J190" s="48"/>
+      <c r="I190" s="41"/>
+      <c r="J190" s="42"/>
     </row>
     <row r="191" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I191" s="47"/>
-      <c r="J191" s="48"/>
+      <c r="I191" s="41"/>
+      <c r="J191" s="42"/>
     </row>
     <row r="192" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I192" s="47"/>
-      <c r="J192" s="48"/>
+      <c r="I192" s="41"/>
+      <c r="J192" s="42"/>
     </row>
     <row r="193" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I193" s="47"/>
-      <c r="J193" s="48"/>
+      <c r="I193" s="41"/>
+      <c r="J193" s="42"/>
     </row>
     <row r="194" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I194" s="47"/>
-      <c r="J194" s="48"/>
+      <c r="I194" s="41"/>
+      <c r="J194" s="42"/>
     </row>
     <row r="195" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I195" s="47"/>
-      <c r="J195" s="48"/>
+      <c r="I195" s="41"/>
+      <c r="J195" s="42"/>
     </row>
     <row r="196" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I196" s="47"/>
-      <c r="J196" s="48"/>
+      <c r="I196" s="41"/>
+      <c r="J196" s="42"/>
     </row>
     <row r="197" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I197" s="47"/>
-      <c r="J197" s="48"/>
+      <c r="I197" s="41"/>
+      <c r="J197" s="42"/>
     </row>
     <row r="198" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I198" s="47"/>
-      <c r="J198" s="48"/>
+      <c r="I198" s="41"/>
+      <c r="J198" s="42"/>
     </row>
     <row r="199" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I199" s="47"/>
-      <c r="J199" s="48"/>
+      <c r="I199" s="41"/>
+      <c r="J199" s="42"/>
     </row>
     <row r="200" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I200" s="47"/>
-      <c r="J200" s="48"/>
+      <c r="I200" s="41"/>
+      <c r="J200" s="42"/>
     </row>
     <row r="201" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I201" s="47"/>
-      <c r="J201" s="48"/>
+      <c r="I201" s="41"/>
+      <c r="J201" s="42"/>
     </row>
     <row r="202" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I202" s="47"/>
-      <c r="J202" s="48"/>
+      <c r="I202" s="41"/>
+      <c r="J202" s="42"/>
     </row>
     <row r="203" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I203" s="47"/>
-      <c r="J203" s="48"/>
+      <c r="I203" s="41"/>
+      <c r="J203" s="42"/>
     </row>
     <row r="204" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I204" s="47"/>
-      <c r="J204" s="48"/>
+      <c r="I204" s="41"/>
+      <c r="J204" s="42"/>
     </row>
     <row r="205" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I205" s="47"/>
-      <c r="J205" s="48"/>
+      <c r="I205" s="41"/>
+      <c r="J205" s="42"/>
     </row>
     <row r="206" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I206" s="47"/>
-      <c r="J206" s="48"/>
+      <c r="I206" s="41"/>
+      <c r="J206" s="42"/>
     </row>
     <row r="207" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I207" s="47"/>
-      <c r="J207" s="48"/>
+      <c r="I207" s="41"/>
+      <c r="J207" s="42"/>
     </row>
     <row r="208" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I208" s="47"/>
-      <c r="J208" s="48"/>
+      <c r="I208" s="41"/>
+      <c r="J208" s="42"/>
     </row>
     <row r="209" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I209" s="47"/>
-      <c r="J209" s="48"/>
+      <c r="I209" s="41"/>
+      <c r="J209" s="42"/>
     </row>
     <row r="210" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I210" s="47"/>
-      <c r="J210" s="48"/>
+      <c r="I210" s="41"/>
+      <c r="J210" s="42"/>
     </row>
     <row r="211" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I211" s="47"/>
-      <c r="J211" s="48"/>
+      <c r="I211" s="41"/>
+      <c r="J211" s="42"/>
     </row>
     <row r="212" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I212" s="47"/>
-      <c r="J212" s="48"/>
+      <c r="I212" s="41"/>
+      <c r="J212" s="42"/>
     </row>
     <row r="213" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I213" s="47"/>
-      <c r="J213" s="48"/>
+      <c r="I213" s="41"/>
+      <c r="J213" s="42"/>
     </row>
     <row r="214" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I214" s="47"/>
-      <c r="J214" s="48"/>
+      <c r="I214" s="41"/>
+      <c r="J214" s="42"/>
     </row>
     <row r="215" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I215" s="47"/>
-      <c r="J215" s="48"/>
+      <c r="I215" s="41"/>
+      <c r="J215" s="42"/>
     </row>
     <row r="216" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I216" s="47"/>
-      <c r="J216" s="48"/>
+      <c r="I216" s="41"/>
+      <c r="J216" s="42"/>
     </row>
     <row r="217" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I217" s="47"/>
-      <c r="J217" s="48"/>
+      <c r="I217" s="41"/>
+      <c r="J217" s="42"/>
     </row>
     <row r="218" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I218" s="47"/>
-      <c r="J218" s="48"/>
+      <c r="I218" s="41"/>
+      <c r="J218" s="42"/>
     </row>
     <row r="219" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I219" s="47"/>
-      <c r="J219" s="48"/>
+      <c r="I219" s="41"/>
+      <c r="J219" s="42"/>
     </row>
     <row r="220" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I220" s="47"/>
-      <c r="J220" s="48"/>
+      <c r="I220" s="41"/>
+      <c r="J220" s="42"/>
     </row>
     <row r="221" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I221" s="47"/>
-      <c r="J221" s="48"/>
+      <c r="I221" s="41"/>
+      <c r="J221" s="42"/>
     </row>
     <row r="222" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I222" s="47"/>
-      <c r="J222" s="48"/>
+      <c r="I222" s="41"/>
+      <c r="J222" s="42"/>
     </row>
     <row r="223" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I223" s="47"/>
-      <c r="J223" s="48"/>
+      <c r="I223" s="41"/>
+      <c r="J223" s="42"/>
     </row>
     <row r="224" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I224" s="47"/>
-      <c r="J224" s="48"/>
+      <c r="I224" s="41"/>
+      <c r="J224" s="42"/>
     </row>
     <row r="225" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I225" s="47"/>
-      <c r="J225" s="48"/>
+      <c r="I225" s="41"/>
+      <c r="J225" s="42"/>
     </row>
     <row r="226" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I226" s="47"/>
-      <c r="J226" s="48"/>
+      <c r="I226" s="41"/>
+      <c r="J226" s="42"/>
     </row>
     <row r="227" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I227" s="47"/>
-      <c r="J227" s="48"/>
+      <c r="I227" s="41"/>
+      <c r="J227" s="42"/>
     </row>
     <row r="228" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I228" s="47"/>
-      <c r="J228" s="48"/>
+      <c r="I228" s="41"/>
+      <c r="J228" s="42"/>
     </row>
     <row r="229" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I229" s="47"/>
-      <c r="J229" s="48"/>
+      <c r="I229" s="41"/>
+      <c r="J229" s="42"/>
     </row>
     <row r="230" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I230" s="47"/>
-      <c r="J230" s="48"/>
+      <c r="I230" s="41"/>
+      <c r="J230" s="42"/>
     </row>
     <row r="231" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I231" s="47"/>
-      <c r="J231" s="48"/>
+      <c r="I231" s="41"/>
+      <c r="J231" s="42"/>
     </row>
     <row r="232" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I232" s="47"/>
-      <c r="J232" s="48"/>
+      <c r="I232" s="41"/>
+      <c r="J232" s="42"/>
     </row>
     <row r="233" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I233" s="47"/>
-      <c r="J233" s="48"/>
+      <c r="I233" s="41"/>
+      <c r="J233" s="42"/>
     </row>
     <row r="234" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I234" s="47"/>
-      <c r="J234" s="48"/>
+      <c r="I234" s="41"/>
+      <c r="J234" s="42"/>
     </row>
     <row r="235" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I235" s="47"/>
-      <c r="J235" s="48"/>
+      <c r="I235" s="41"/>
+      <c r="J235" s="42"/>
     </row>
     <row r="236" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I236" s="47"/>
-      <c r="J236" s="48"/>
+      <c r="I236" s="41"/>
+      <c r="J236" s="42"/>
     </row>
     <row r="237" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I237" s="47"/>
-      <c r="J237" s="48"/>
+      <c r="I237" s="41"/>
+      <c r="J237" s="42"/>
     </row>
     <row r="238" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I238" s="47"/>
-      <c r="J238" s="48"/>
+      <c r="I238" s="41"/>
+      <c r="J238" s="42"/>
     </row>
     <row r="239" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I239" s="47"/>
-      <c r="J239" s="48"/>
+      <c r="I239" s="41"/>
+      <c r="J239" s="42"/>
     </row>
     <row r="240" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I240" s="47"/>
-      <c r="J240" s="48"/>
+      <c r="I240" s="41"/>
+      <c r="J240" s="42"/>
     </row>
     <row r="241" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I241" s="47"/>
-      <c r="J241" s="48"/>
+      <c r="I241" s="41"/>
+      <c r="J241" s="42"/>
     </row>
     <row r="242" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I242" s="47"/>
-      <c r="J242" s="48"/>
+      <c r="I242" s="41"/>
+      <c r="J242" s="42"/>
     </row>
     <row r="243" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I243" s="47"/>
-      <c r="J243" s="48"/>
+      <c r="I243" s="41"/>
+      <c r="J243" s="42"/>
     </row>
     <row r="244" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I244" s="47"/>
-      <c r="J244" s="48"/>
+      <c r="I244" s="41"/>
+      <c r="J244" s="42"/>
     </row>
     <row r="245" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I245" s="47"/>
-      <c r="J245" s="48"/>
+      <c r="I245" s="41"/>
+      <c r="J245" s="42"/>
     </row>
     <row r="246" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I246" s="47"/>
-      <c r="J246" s="48"/>
+      <c r="I246" s="41"/>
+      <c r="J246" s="42"/>
     </row>
     <row r="247" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I247" s="47"/>
-      <c r="J247" s="48"/>
+      <c r="I247" s="41"/>
+      <c r="J247" s="42"/>
     </row>
     <row r="248" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I248" s="47"/>
-      <c r="J248" s="48"/>
+      <c r="I248" s="41"/>
+      <c r="J248" s="42"/>
     </row>
     <row r="249" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I249" s="47"/>
-      <c r="J249" s="48"/>
+      <c r="I249" s="41"/>
+      <c r="J249" s="42"/>
     </row>
     <row r="250" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I250" s="47"/>
-      <c r="J250" s="48"/>
+      <c r="I250" s="41"/>
+      <c r="J250" s="42"/>
     </row>
     <row r="251" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I251" s="47"/>
-      <c r="J251" s="48"/>
+      <c r="I251" s="41"/>
+      <c r="J251" s="42"/>
     </row>
     <row r="252" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I252" s="47"/>
-      <c r="J252" s="48"/>
+      <c r="I252" s="41"/>
+      <c r="J252" s="42"/>
     </row>
     <row r="253" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I253" s="47"/>
-      <c r="J253" s="48"/>
+      <c r="I253" s="41"/>
+      <c r="J253" s="42"/>
     </row>
     <row r="254" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I254" s="47"/>
-      <c r="J254" s="48"/>
+      <c r="I254" s="41"/>
+      <c r="J254" s="42"/>
     </row>
     <row r="255" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I255" s="47"/>
-      <c r="J255" s="48"/>
+      <c r="I255" s="41"/>
+      <c r="J255" s="42"/>
     </row>
     <row r="256" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I256" s="47"/>
-      <c r="J256" s="48"/>
+      <c r="I256" s="41"/>
+      <c r="J256" s="42"/>
     </row>
     <row r="257" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I257" s="47"/>
-      <c r="J257" s="48"/>
+      <c r="I257" s="41"/>
+      <c r="J257" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -7652,7 +7627,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>